<commit_message>
Add new CSV files for ticket data and update product pricing in existing files
</commit_message>
<xml_diff>
--- a/Transacciones_Excel.xlsx
+++ b/Transacciones_Excel.xlsx
@@ -495,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45416.01805550183</v>
+        <v>45400.70097197202</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -512,11 +512,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>Completado</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>88.45999999999999</v>
+        <v>151.97</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -524,23 +524,19 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Sin observaciones</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45583.01805550183</v>
+        <v>45509.70097197202</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -558,7 +554,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>171.96</v>
+        <v>139.93</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -566,7 +562,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" t="inlineStr"/>
     </row>
@@ -578,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45460.01805550183</v>
+        <v>45490.70097197202</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -592,11 +588,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>En proceso</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>152.3</v>
+        <v>95.84</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -604,7 +600,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -617,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45525.01805550183</v>
+        <v>45529.70097197202</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -634,11 +630,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>En proceso</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>31.44</v>
+        <v>141.76</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -646,23 +642,19 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Observado</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45318.01805550183</v>
+        <v>45417.70097197202</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -680,7 +672,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>174.72</v>
+        <v>195.52</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -688,7 +680,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr"/>
     </row>
@@ -697,10 +689,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45564.01805550183</v>
+        <v>45490.70097197202</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -714,11 +706,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>En proceso</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>113.28</v>
+        <v>16.09</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -726,23 +718,19 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>9</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Sin observaciones</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45550.01805550183</v>
+        <v>45340.70097197202</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -756,11 +744,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>En proceso</t>
+          <t>Rechazado</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>37.24</v>
+        <v>165.47</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -768,11 +756,11 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Observado</t>
+          <t>Sin observaciones</t>
         </is>
       </c>
     </row>
@@ -781,10 +769,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45582.01805550183</v>
+        <v>45413.70097197202</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -802,7 +790,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>121.23</v>
+        <v>185.56</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -810,23 +798,19 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>7</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Sin observaciones</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45542.01805550183</v>
+        <v>45317.70097197202</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -844,7 +828,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>153.52</v>
+        <v>182.74</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -852,11 +836,11 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Observado</t>
+          <t>Sin observaciones</t>
         </is>
       </c>
     </row>
@@ -865,42 +849,38 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45375.70097197202</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Venta</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OP000010</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Rechazado</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>177.13</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Soles</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>45309.01805550183</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Venta</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>OP000010</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>En proceso</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>167.09</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Soles</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>3</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Sin observaciones</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -910,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45258.01805550183</v>
+        <v>45619.70097197202</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -924,11 +904,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Completado</t>
+          <t>En proceso</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>19.74</v>
+        <v>51.76</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -936,7 +916,7 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J12" t="inlineStr"/>
     </row>
@@ -945,36 +925,36 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45463.70097197202</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Venta</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OP000012</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>En proceso</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Soles</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
         <v>2</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>45561.01805550183</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Venta</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>OP000012</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>En proceso</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>132.23</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Soles</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -987,10 +967,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45319.01805550183</v>
+        <v>45363.70097197202</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1008,7 +988,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>53.31</v>
+        <v>56.19</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1016,11 +996,11 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Sin observaciones</t>
+          <t>Observado</t>
         </is>
       </c>
     </row>
@@ -1029,10 +1009,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45570.01805550183</v>
+        <v>45556.70097197202</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1046,11 +1026,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>En proceso</t>
+          <t>Completado</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>121.56</v>
+        <v>148.74</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1058,19 +1038,23 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>9</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Observado</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45416.01805550183</v>
+        <v>45591.70097197202</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1088,7 +1072,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>139.33</v>
+        <v>101.61</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1096,23 +1080,19 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>7</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Sin observaciones</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45520.01805550183</v>
+        <v>45501.70097197202</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1130,7 +1110,7 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>9.710000000000001</v>
+        <v>87.33</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1147,10 +1127,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45573.01805550183</v>
+        <v>45309.70097197202</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1168,7 +1148,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>69.05</v>
+        <v>13.44</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1176,11 +1156,11 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Sin observaciones</t>
+          <t>Observado</t>
         </is>
       </c>
     </row>
@@ -1192,7 +1172,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45558.01805550183</v>
+        <v>45481.70097197202</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1210,7 +1190,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>57.42</v>
+        <v>145.83</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1218,23 +1198,19 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>7</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Observado</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45518.01805550183</v>
+        <v>45601.70097197202</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1248,11 +1224,11 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Completado</t>
+          <t>En proceso</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>153.06</v>
+        <v>13.52</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1260,13 +1236,9 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>4</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Observado</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1276,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45502.01805550183</v>
+        <v>45282.70097197202</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1290,11 +1262,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Rechazado</t>
+          <t>Completado</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>138.12</v>
+        <v>33.44</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1302,13 +1274,9 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>5</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Observado</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1369,16 +1337,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>8.57</v>
+        <v>4.33</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.89</v>
+        <v>3.71</v>
       </c>
       <c r="F2" t="n">
-        <v>2.76</v>
+        <v>14.56</v>
       </c>
     </row>
     <row r="3">
@@ -1389,16 +1357,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>12.06</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.24</v>
+        <v>9.76</v>
       </c>
       <c r="F3" t="n">
-        <v>5.24</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="4">
@@ -1409,16 +1377,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>15.57</v>
+        <v>4.57</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>9.77</v>
+        <v>0.46</v>
       </c>
       <c r="F4" t="n">
-        <v>2.32</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="5">
@@ -1429,16 +1397,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>3.33</v>
+        <v>0.93</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>3.8</v>
       </c>
       <c r="F5" t="n">
-        <v>6.36</v>
+        <v>9.390000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -1449,16 +1417,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>12.98</v>
+        <v>10.35</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>8.84</v>
+        <v>0.91</v>
       </c>
       <c r="F6" t="n">
-        <v>3.34</v>
+        <v>9.539999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -1469,16 +1437,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.01</v>
+        <v>10.22</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>1.84</v>
+        <v>3.28</v>
       </c>
       <c r="F7" t="n">
-        <v>9.81</v>
+        <v>5.73</v>
       </c>
     </row>
     <row r="8">
@@ -1489,16 +1457,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>19.76</v>
+        <v>1.25</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.77</v>
+        <v>3.48</v>
       </c>
       <c r="F8" t="n">
-        <v>4.56</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="9">
@@ -1509,16 +1477,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>14.45</v>
+        <v>4.18</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>5.41</v>
+        <v>9.6</v>
       </c>
       <c r="F9" t="n">
-        <v>3.52</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="10">
@@ -1529,16 +1497,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>4.61</v>
+        <v>6.22</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>3.33</v>
+        <v>7.18</v>
       </c>
       <c r="F10" t="n">
-        <v>11.11</v>
+        <v>11.48</v>
       </c>
     </row>
     <row r="11">
@@ -1549,16 +1517,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>15.39</v>
+        <v>10.17</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.74</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="F11" t="n">
-        <v>6.5</v>
+        <v>11.17</v>
       </c>
     </row>
     <row r="12">
@@ -1569,16 +1537,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>11.9</v>
+        <v>17.14</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>4.64</v>
+        <v>7.55</v>
       </c>
       <c r="F12" t="n">
-        <v>3.73</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="13">
@@ -1589,16 +1557,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>10.61</v>
+        <v>3.83</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>4.37</v>
+        <v>0.92</v>
       </c>
       <c r="F13" t="n">
-        <v>13.28</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -1609,16 +1577,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>17.09</v>
+        <v>0.3</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>7.84</v>
+        <v>7.45</v>
       </c>
       <c r="F14" t="n">
-        <v>10.54</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="15">
@@ -1629,16 +1597,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>12.58</v>
+        <v>3.46</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>3.95</v>
+        <v>4.06</v>
       </c>
       <c r="F15" t="n">
-        <v>2.06</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="16">
@@ -1649,16 +1617,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>7.46</v>
+        <v>15.1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>5.52</v>
+        <v>0.87</v>
       </c>
       <c r="F16" t="n">
-        <v>5.94</v>
+        <v>10.23</v>
       </c>
     </row>
     <row r="17">
@@ -1669,16 +1637,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>17.15</v>
+        <v>1.44</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>8.789999999999999</v>
+        <v>5.92</v>
       </c>
       <c r="F17" t="n">
-        <v>12.08</v>
+        <v>13.55</v>
       </c>
     </row>
     <row r="18">
@@ -1689,16 +1657,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>5.76</v>
+        <v>5.33</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>3.69</v>
+        <v>1.99</v>
       </c>
       <c r="F18" t="n">
-        <v>6.86</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="19">
@@ -1709,16 +1677,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>13.42</v>
+        <v>13.77</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>8.59</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="20">
@@ -1729,16 +1697,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>3.99</v>
       </c>
       <c r="F20" t="n">
-        <v>0.34</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="21">
@@ -1749,16 +1717,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>18.68</v>
+        <v>11.76</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>4.53</v>
+        <v>3.65</v>
       </c>
       <c r="F21" t="n">
-        <v>0.45</v>
+        <v>6.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>